<commit_message>
add isHandValve, IsControlValve, Safety and Blowdown columns
</commit_message>
<xml_diff>
--- a/Waterfall 3.0 to 3.6.xlsx
+++ b/Waterfall 3.0 to 3.6.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="0" windowWidth="27870" windowHeight="11295" activeTab="2"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="27870" windowHeight="11295"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
@@ -5011,6 +5011,28 @@
             <a:t>3.4 - Make F&amp;G Detector failure codes A</a:t>
           </a:r>
         </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>3.5 - Split lighting into hig/medium/low (aligns with systems at this stage)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>3.6 - Make SIL input/output tags A  (only affects 6 not caught by shutdown tag above)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -5417,7 +5439,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
@@ -8804,7 +8826,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Q112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="Q109" sqref="Q109"/>
     </sheetView>
   </sheetViews>

</xml_diff>